<commit_message>
Active account balance report Excel & Cash Report
</commit_message>
<xml_diff>
--- a/admin/ACTIVE_ACCOUNT_BALANCE_REPORT.xlsx
+++ b/admin/ACTIVE_ACCOUNT_BALANCE_REPORT.xlsx
@@ -15,45 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>ACTIVE ACCOUNT BALANCE REPORT</t>
   </si>
   <si>
-    <t>Range 1</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Service Code</t>
-  </si>
-  <si>
-    <t>Enroll</t>
-  </si>
-  <si>
-    <t>Used</t>
-  </si>
-  <si>
-    <t>Scheduled</t>
-  </si>
-  <si>
-    <t>Remain</t>
-  </si>
-  <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>Paid</t>
-  </si>
-  <si>
-    <t>PRI1</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>PRT</t>
+    <t>Date 08-06-2025</t>
   </si>
 </sst>
 </file>
@@ -439,10 +406,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,126 +452,44 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5">
-        <v>60</v>
-      </c>
-      <c r="D4" s="5">
-        <v>41</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5">
-        <v>4</v>
-      </c>
-      <c r="H4" s="5">
-        <v>7229.25</v>
-      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5">
-        <v>185</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2</v>
-      </c>
-      <c r="G7" s="5">
-        <v>2</v>
-      </c>
-      <c r="H7" s="5">
-        <v>180</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>